<commit_message>
language of test report documents changed (to eng)
</commit_message>
<xml_diff>
--- a/test/DefectTable.xlsx
+++ b/test/DefectTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Defect id</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>ManualTest28042014 - Test Case 5/10/13</t>
+  </si>
+  <si>
+    <t>Resolved on</t>
   </si>
 </sst>
 </file>
@@ -407,22 +410,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,19 +437,22 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -455,20 +462,20 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>41757</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -478,20 +485,20 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>41757</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -501,21 +508,21 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>41757</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="G5" t="s">
+    <row r="5" spans="1:8">
+      <c r="H5" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new defect found and added to defect table (D4)
</commit_message>
<xml_diff>
--- a/test/DefectTable.xlsx
+++ b/test/DefectTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Defect id</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>Resolved on</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>Events that already have tweets cannot be deleted.</t>
   </si>
 </sst>
 </file>
@@ -112,10 +118,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -526,6 +533,26 @@
         <v>17</v>
       </c>
     </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1">
+        <v>41759</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add defect to defect table
</commit_message>
<xml_diff>
--- a/test/DefectTable.xlsx
+++ b/test/DefectTable.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>Defect id</t>
   </si>
@@ -167,13 +167,19 @@
   </si>
   <si>
     <t>Update 28.5.: special character " now is also cut on event name.</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>Saving events without Date from and Date to is possible and gives false saved dates: 30.11.-0001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -373,19 +379,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -423,7 +436,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -457,6 +470,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -491,9 +505,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -666,14 +681,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="C23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="9" customWidth="1"/>
@@ -684,7 +699,7 @@
     <col min="9" max="9" width="119.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -751,11 +766,11 @@
       <c r="U2" s="4"/>
       <c r="V2" s="7"/>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:22" s="14" customFormat="1">
+    <row r="4" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -780,7 +795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="14" customFormat="1">
+    <row r="5" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="30"/>
@@ -793,11 +808,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -824,7 +839,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -837,7 +852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -856,7 +871,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -881,7 +896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -906,7 +921,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>30</v>
       </c>
@@ -931,7 +946,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -944,7 +959,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -955,7 +970,7 @@
       <c r="H17" s="17"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -980,7 +995,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>34</v>
       </c>
@@ -1005,7 +1020,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -1018,10 +1033,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>38</v>
       </c>
@@ -1040,7 +1055,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
         <v>43</v>
       </c>
@@ -1063,10 +1078,10 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>45</v>
       </c>
@@ -1087,7 +1102,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -1100,8 +1115,31 @@
         <v>48</v>
       </c>
     </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="1">
+        <v>41794</v>
+      </c>
+      <c r="G31" s="34">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="33"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
defect table commited docu screenshots added to repo
</commit_message>
<xml_diff>
--- a/test/DefectTable.xlsx
+++ b/test/DefectTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
   <si>
     <t>Defect id</t>
   </si>
@@ -73,9 +73,6 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Events that already have tweets cannot be deleted.</t>
-  </si>
-  <si>
     <t>Update to D3 - as of 14.05., the right date format is now shown on editing.</t>
   </si>
   <si>
@@ -200,13 +197,34 @@
   </si>
   <si>
     <t>Update 4.6.: exception also occurs when filled into the filter name property. Exception does now not occur on location property, but text is not shown.</t>
+  </si>
+  <si>
+    <t>manfred</t>
+  </si>
+  <si>
+    <t>andreas</t>
+  </si>
+  <si>
+    <t>Events that already have tweets cannot be deleted. Expected: the right error message (e.g. "not deletable") or cascading delete.</t>
+  </si>
+  <si>
+    <t>followup</t>
+  </si>
+  <si>
+    <t>nicht unterstützt</t>
+  </si>
+  <si>
+    <t>No Defect</t>
+  </si>
+  <si>
+    <t>to be documented. Works with clicking on search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +252,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -372,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -408,6 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,18 +735,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="142.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -735,7 +763,7 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -763,7 +791,9 @@
       <c r="C2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="5">
         <v>41757</v>
@@ -772,7 +802,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>6</v>
@@ -805,7 +835,9 @@
       <c r="C4" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="E4" s="9"/>
       <c r="F4" s="10">
         <v>41757</v>
@@ -814,7 +846,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="12" t="s">
         <v>10</v>
@@ -830,7 +862,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="17"/>
       <c r="I5" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -845,7 +877,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10">
@@ -858,7 +890,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>16</v>
@@ -890,10 +922,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -906,7 +938,9 @@
       <c r="C11" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="5">
         <v>41759</v>
@@ -915,23 +949,25 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="5">
         <v>41773</v>
@@ -940,15 +976,15 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="H13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>8</v>
@@ -956,7 +992,9 @@
       <c r="C15" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="E15" s="9"/>
       <c r="F15" s="10">
         <v>41773</v>
@@ -965,10 +1003,10 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -981,10 +1019,10 @@
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="16"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -994,12 +1032,12 @@
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>8</v>
@@ -1016,15 +1054,18 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>47</v>
+      </c>
+      <c r="J19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>12</v>
@@ -1041,13 +1082,16 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>34</v>
+      </c>
+      <c r="J21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="25"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -1057,22 +1101,22 @@
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
       <c r="I22" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="23"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="26" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="23"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="26" t="s">
-        <v>38</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="5">
         <v>41794</v>
@@ -1081,21 +1125,21 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="5">
@@ -1104,15 +1148,15 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="23"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="8" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="23"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>8</v>
@@ -1120,7 +1164,9 @@
       <c r="C28" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="9"/>
+      <c r="D28" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="E28" s="9"/>
       <c r="F28" s="10">
         <v>41780</v>
@@ -1128,10 +1174,10 @@
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="16"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -1141,12 +1187,12 @@
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
       <c r="I29" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>12</v>
@@ -1154,7 +1200,9 @@
       <c r="C31" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="E31" s="4"/>
       <c r="F31" s="5">
         <v>41794</v>
@@ -1164,15 +1212,15 @@
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="C32" s="33"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="C32" s="33"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>8</v>
@@ -1180,7 +1228,9 @@
       <c r="C33" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="E33" s="4"/>
       <c r="F33" s="5">
         <v>41794</v>
@@ -1189,15 +1239,15 @@
         <v>0.625</v>
       </c>
       <c r="H33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I33" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I33" s="7" t="s">
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="3" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>8</v>
@@ -1205,7 +1255,9 @@
       <c r="C35" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="4"/>
+      <c r="D35" s="35" t="s">
+        <v>66</v>
+      </c>
       <c r="E35" s="4"/>
       <c r="F35" s="5">
         <v>41794</v>
@@ -1214,15 +1266,18 @@
         <v>0.625</v>
       </c>
       <c r="H35" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="J35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="3" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>12</v>
@@ -1230,7 +1285,9 @@
       <c r="C37" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="4"/>
+      <c r="D37" s="35" t="s">
+        <v>45</v>
+      </c>
       <c r="E37" s="4"/>
       <c r="F37" s="5">
         <v>41794</v>
@@ -1239,10 +1296,10 @@
         <v>0.625</v>
       </c>
       <c r="H37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I37" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
defect table with verified / updated
</commit_message>
<xml_diff>
--- a/test/DefectTable.xlsx
+++ b/test/DefectTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t>Defect id</t>
   </si>
@@ -100,9 +100,6 @@
     <t>ManualTest14052014 - TestCase 3-4</t>
   </si>
   <si>
-    <t>Sometimes when choosing an event and a filter, and then choosing another event, the tweets table is not updated.</t>
-  </si>
-  <si>
     <t>D6</t>
   </si>
   <si>
@@ -211,13 +208,40 @@
     <t>followup</t>
   </si>
   <si>
-    <t>nicht unterstützt</t>
-  </si>
-  <si>
     <t>No Defect</t>
   </si>
   <si>
     <t>to be documented. Works with clicking on search</t>
+  </si>
+  <si>
+    <t>Update 11.6.: special characters cannot be inserted into text fields (only into event description)</t>
+  </si>
+  <si>
+    <t>Update 11.6. text fields are now restricted in the amount of text.</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>Update 11.6.: dates cannot be set in the past (intended?)</t>
+  </si>
+  <si>
+    <t>When choosing an event and a filter, and then choosing another event, the tweets table is not updated.</t>
+  </si>
+  <si>
+    <t>Update 11.6.: special characters cannot be inserted anymore.</t>
+  </si>
+  <si>
+    <t>Update 11.6.: Text fields are now restricted</t>
+  </si>
+  <si>
+    <t>not supported anymore</t>
+  </si>
+  <si>
+    <t>Update 11.6.: deleted tweets are still considered for analysis.</t>
+  </si>
+  <si>
+    <t>Ignored tweets are not considered for analysis when ignored - OK. But after toggling the ignore-status off (when it was on), the tweets are still not considered.</t>
   </si>
 </sst>
 </file>
@@ -268,7 +292,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -393,11 +417,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -432,8 +497,16 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V37"/>
+  <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="I19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -749,7 +822,8 @@
     <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="142.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="152.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -763,7 +837,7 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -792,7 +866,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="5">
@@ -804,7 +878,7 @@
       <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="4"/>
@@ -822,484 +896,588 @@
       <c r="V2" s="7"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:22" s="14" customFormat="1">
-      <c r="A4" s="8" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="F4" s="1"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" s="14" customFormat="1">
+      <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C5" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10">
+        <v>41757</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="14" customFormat="1">
+      <c r="A6" s="13"/>
+      <c r="C6" s="35"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="37"/>
+      <c r="I6" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="14" customFormat="1">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="F8" s="1"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10">
+        <v>41787</v>
+      </c>
+      <c r="F9" s="10">
+        <v>41757</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="24">
+        <v>41773</v>
+      </c>
+      <c r="G12" s="18">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5">
+        <v>41759</v>
+      </c>
+      <c r="G14" s="20">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10">
-        <v>41757</v>
-      </c>
-      <c r="G4" s="11">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" s="14" customFormat="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="9" t="s">
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5">
+        <v>41773</v>
+      </c>
+      <c r="G16" s="20">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10">
+        <v>41773</v>
+      </c>
+      <c r="G18" s="22">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5">
+        <v>41773</v>
+      </c>
+      <c r="G23" s="20">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10">
-        <v>41787</v>
-      </c>
-      <c r="F7" s="10">
-        <v>41757</v>
-      </c>
-      <c r="G7" s="11">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="24">
+      <c r="C26" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10">
         <v>41773</v>
       </c>
-      <c r="G9" s="18">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5">
-        <v>41759</v>
-      </c>
-      <c r="G11" s="20">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="A13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="G26" s="22">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="25"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="23"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="5">
+        <v>41794</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5">
-        <v>41773</v>
-      </c>
-      <c r="G13" s="20">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
-      <c r="A15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10">
-        <v>41773</v>
-      </c>
-      <c r="G15" s="22">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5">
-        <v>41773</v>
-      </c>
-      <c r="G19" s="20">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10">
-        <v>41773</v>
-      </c>
-      <c r="G21" s="22">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="25"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="23"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="5">
-        <v>41794</v>
-      </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="7" t="s">
+      <c r="C31" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="5">
-        <v>41780</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="23"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="10">
-        <v>41780</v>
-      </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="16"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="5">
-        <v>41794</v>
-      </c>
-      <c r="G31" s="20">
-        <v>0.41666666666666669</v>
-      </c>
+        <v>41780</v>
+      </c>
+      <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="23"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="10">
+        <v>41780</v>
+      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="5">
+        <v>41794</v>
+      </c>
+      <c r="G36" s="20">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H36" s="4"/>
+      <c r="I36" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="C37" s="33"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="C32" s="33"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="3" t="s">
+      <c r="B38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="5">
+        <v>41794</v>
+      </c>
+      <c r="G38" s="20">
+        <v>0.625</v>
+      </c>
+      <c r="H38" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="I38" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C40" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="5">
+        <v>41794</v>
+      </c>
+      <c r="G40" s="20">
+        <v>0.625</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="5">
+      <c r="D42" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="5">
         <v>41794</v>
       </c>
-      <c r="G33" s="20">
+      <c r="G42" s="20">
         <v>0.625</v>
       </c>
-      <c r="H33" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="5">
-        <v>41794</v>
-      </c>
-      <c r="G35" s="20">
-        <v>0.625</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="3" t="s">
+      <c r="H42" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="5">
-        <v>41794</v>
-      </c>
-      <c r="G37" s="20">
-        <v>0.625</v>
-      </c>
-      <c r="H37" s="4" t="s">
+      <c r="I42" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I37" s="7" t="s">
-        <v>59</v>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="13"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="16"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="32" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
many small fixed checked in user docu & qaplan updated
</commit_message>
<xml_diff>
--- a/test/DefectTable.xlsx
+++ b/test/DefectTable.xlsx
@@ -811,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
defect table camera ready
</commit_message>
<xml_diff>
--- a/test/DefectTable.xlsx
+++ b/test/DefectTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
   <si>
     <t>Defect id</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>False values are saved, and a false format of date values is shown in the editing.</t>
   </si>
   <si>
@@ -148,9 +145,6 @@
     <t>Date to can be before Date from</t>
   </si>
   <si>
-    <t>resolved</t>
-  </si>
-  <si>
     <t>Update 28.5.: dates can now be selected with a calendar. Still, Date to can be before date from.</t>
   </si>
   <si>
@@ -242,16 +236,13 @@
   </si>
   <si>
     <t>Ignored tweets are not considered for analysis when ignored - OK. But after toggling the ignore-status off (when it was on), the tweets are still not considered.</t>
-  </si>
-  <si>
-    <t>not resolved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,13 +259,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -465,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -493,19 +477,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -811,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -840,10 +821,10 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -865,11 +846,11 @@
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>44</v>
+      <c r="C2" s="31" t="s">
+        <v>66</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="5">
@@ -879,7 +860,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>6</v>
@@ -901,14 +882,14 @@
     <row r="3" spans="1:22">
       <c r="A3" s="16"/>
       <c r="B3" s="17"/>
-      <c r="C3" s="30"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="24"/>
-      <c r="G3" s="31"/>
+      <c r="G3" s="28"/>
       <c r="H3" s="17"/>
       <c r="I3" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
@@ -935,11 +916,11 @@
       <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>44</v>
+      <c r="C5" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="10">
@@ -949,7 +930,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>10</v>
@@ -957,24 +938,24 @@
     </row>
     <row r="6" spans="1:22" s="14" customFormat="1">
       <c r="A6" s="13"/>
-      <c r="C6" s="35"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="37"/>
+      <c r="C6" s="32"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
       <c r="I6" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="14" customFormat="1">
       <c r="A7" s="16"/>
       <c r="B7" s="17"/>
-      <c r="C7" s="30"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="24"/>
-      <c r="G7" s="31"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="17"/>
-      <c r="I7" s="32" t="s">
-        <v>66</v>
+      <c r="I7" s="29" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -988,8 +969,8 @@
       <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>44</v>
+      <c r="C9" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="10">
@@ -1002,10 +983,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -1018,7 +999,7 @@
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -1031,7 +1012,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -1047,24 +1028,24 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="28" t="s">
-        <v>44</v>
+      <c r="C14" s="31" t="s">
+        <v>66</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="5">
@@ -1074,24 +1055,24 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>44</v>
+      <c r="C16" s="31" t="s">
+        <v>66</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="5">
@@ -1101,24 +1082,24 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="38" t="s">
-        <v>68</v>
+      <c r="C18" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="10">
@@ -1128,10 +1109,10 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1144,7 +1125,7 @@
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1157,7 +1138,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1170,18 +1151,18 @@
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
       <c r="I21" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="34" t="s">
-        <v>68</v>
+      <c r="C23" s="31" t="s">
+        <v>66</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1192,37 +1173,37 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="16"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="39"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
       <c r="F24" s="24"/>
       <c r="G24" s="18"/>
       <c r="H24" s="17"/>
-      <c r="I24" s="32" t="s">
-        <v>72</v>
+      <c r="I24" s="29" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="38" t="s">
-        <v>68</v>
+      <c r="C26" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -1233,13 +1214,13 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I26" s="40" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="I26" s="37" t="s">
+        <v>32</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1251,8 +1232,8 @@
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
-      <c r="I27" s="41" t="s">
-        <v>35</v>
+      <c r="I27" s="38" t="s">
+        <v>34</v>
       </c>
       <c r="J27" s="19"/>
     </row>
@@ -1261,14 +1242,14 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="4"/>
-      <c r="C29" s="34" t="s">
-        <v>68</v>
+      <c r="C29" s="31" t="s">
+        <v>66</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" s="5">
         <v>41794</v>
@@ -1277,21 +1258,21 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>68</v>
+        <v>25</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>66</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="5">
@@ -1300,7 +1281,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1308,16 +1289,16 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="38" t="s">
-        <v>68</v>
+      <c r="C33" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="10">
@@ -1326,7 +1307,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1339,21 +1320,21 @@
       <c r="G34" s="17"/>
       <c r="H34" s="17"/>
       <c r="I34" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="28" t="s">
-        <v>44</v>
+      <c r="C36" s="31" t="s">
+        <v>66</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="5">
@@ -1364,24 +1345,24 @@
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="C37" s="33"/>
+      <c r="C37" s="30"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="34" t="s">
-        <v>68</v>
+      <c r="C38" s="31" t="s">
+        <v>66</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="5">
@@ -1391,27 +1372,27 @@
         <v>0.625</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I38" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="I38" s="39" t="s">
+        <v>50</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>64</v>
+      <c r="C40" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>62</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="5">
@@ -1421,27 +1402,27 @@
         <v>0.625</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I40" s="42" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="I40" s="39" t="s">
+        <v>53</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="34" t="s">
-        <v>44</v>
+      <c r="C42" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="5">
@@ -1451,10 +1432,10 @@
         <v>0.625</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1462,14 +1443,14 @@
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
       <c r="D43" s="35" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
       <c r="H43" s="14"/>
-      <c r="I43" s="43" t="s">
-        <v>74</v>
+      <c r="I43" s="40" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1481,8 +1462,8 @@
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
-      <c r="I44" s="32" t="s">
-        <v>75</v>
+      <c r="I44" s="29" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>